<commit_message>
update Column Definition Document
</commit_message>
<xml_diff>
--- a/data/컬럼정의서2.xlsx
+++ b/data/컬럼정의서2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\DS Projects\miniproject1-nycflights\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\flights-project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20355" windowHeight="8805"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20360" windowHeight="8810"/>
   </bookViews>
   <sheets>
     <sheet name="flights" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="173">
   <si>
     <t>컬럼명</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -141,7 +141,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -160,7 +160,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -184,7 +184,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -203,7 +203,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -227,7 +227,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -246,7 +246,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -270,7 +270,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -289,7 +289,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -313,7 +313,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -332,7 +332,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -351,7 +351,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -375,7 +375,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -394,7 +394,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -413,7 +413,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -437,7 +437,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -456,7 +456,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -480,7 +480,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -499,7 +499,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -534,7 +534,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -553,7 +553,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -572,7 +572,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -591,7 +591,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -607,7 +607,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -626,7 +626,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -645,7 +645,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -675,7 +675,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -694,7 +694,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -713,7 +713,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -732,7 +732,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -751,7 +751,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -847,7 +847,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -866,7 +866,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -904,7 +904,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -923,7 +923,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -961,7 +961,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -980,7 +980,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -999,7 +999,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -1159,7 +1159,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -1222,7 +1222,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -1238,6 +1238,153 @@
   <si>
     <t>결측값이 많음</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dep_time</t>
+  </si>
+  <si>
+    <t>sched_dep_time</t>
+  </si>
+  <si>
+    <t>dep_delay</t>
+  </si>
+  <si>
+    <t>arr_time</t>
+  </si>
+  <si>
+    <t>sched_arr_time</t>
+  </si>
+  <si>
+    <t>arr_delay</t>
+  </si>
+  <si>
+    <t>flight</t>
+  </si>
+  <si>
+    <t>tailnum</t>
+  </si>
+  <si>
+    <t>dest</t>
+  </si>
+  <si>
+    <t>air_time</t>
+  </si>
+  <si>
+    <t>distance</t>
+  </si>
+  <si>
+    <t>minute</t>
+  </si>
+  <si>
+    <t>출발 연도</t>
+  </si>
+  <si>
+    <t>출발 월</t>
+  </si>
+  <si>
+    <t>출발 일</t>
+  </si>
+  <si>
+    <t>실제 출발 시각 (HHMM/HMM)</t>
+  </si>
+  <si>
+    <t>예정 출발 시각 (HHMM/HMM)</t>
+  </si>
+  <si>
+    <t>출발 지연(분)</t>
+  </si>
+  <si>
+    <t>실제 도착 시각 (HHMM/HMM)</t>
+  </si>
+  <si>
+    <t>예정 도착 시각 (HHMM/HMM)</t>
+  </si>
+  <si>
+    <t>도착 지연(분)</t>
+  </si>
+  <si>
+    <t>항공편 번호</t>
+  </si>
+  <si>
+    <t>항공기 꼬리 번호</t>
+  </si>
+  <si>
+    <t>출발 공항 FAA 코드</t>
+  </si>
+  <si>
+    <t>도착 공항 FAA 코드</t>
+  </si>
+  <si>
+    <t>실제 비행 시간(분)</t>
+  </si>
+  <si>
+    <t>거리(마일)</t>
+  </si>
+  <si>
+    <t>예정 출발 시각 시(hour)</t>
+  </si>
+  <si>
+    <t>예정 출발 시각 분(minute)</t>
+  </si>
+  <si>
+    <t>예정 출발 날짜 및 시간 (시 단위)</t>
+  </si>
+  <si>
+    <t>2013</t>
+  </si>
+  <si>
+    <t>1, 6, 12</t>
+  </si>
+  <si>
+    <t>1, 15, 31</t>
+  </si>
+  <si>
+    <t>517.0, 533.0, 542.0</t>
+  </si>
+  <si>
+    <t>500, 505, 510</t>
+  </si>
+  <si>
+    <t>-5.0, 0.0, 10.0</t>
+  </si>
+  <si>
+    <t>845.0, 1312.0, 2203.0</t>
+  </si>
+  <si>
+    <t>845, 1315, 2210</t>
+  </si>
+  <si>
+    <t>-3.0, 0.0, 15.0</t>
+  </si>
+  <si>
+    <t>'AA', 'DL', 'UA'</t>
+  </si>
+  <si>
+    <t>1, 8, 215</t>
+  </si>
+  <si>
+    <t>'N10156', 'N102UW', 'N103US'</t>
+  </si>
+  <si>
+    <t>'JFK', 'LGA', 'EWR'</t>
+  </si>
+  <si>
+    <t>'LAX', 'ORD', 'MIA'</t>
+  </si>
+  <si>
+    <t>30.0, 150.0, 360.0</t>
+  </si>
+  <si>
+    <t>108, 1432, 2475</t>
+  </si>
+  <si>
+    <t>5, 12, 17</t>
+  </si>
+  <si>
+    <t>0, 15, 30</t>
+  </si>
+  <si>
+    <t>2013-01-01 05:00, 2013-06-15 14:00, 2013-12-31 23:00</t>
   </si>
 </sst>
 </file>
@@ -1248,14 +1395,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1268,7 +1415,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="major"/>
@@ -1620,15 +1767,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="3" max="3" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="42" customHeight="1">
@@ -1658,6 +1803,443 @@
       </c>
       <c r="I1" s="9" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2">
+        <v>336776</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3">
+        <v>336776</v>
+      </c>
+      <c r="E3">
+        <v>12</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4">
+        <v>336776</v>
+      </c>
+      <c r="E4">
+        <v>31</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5">
+        <v>336776</v>
+      </c>
+      <c r="E5">
+        <v>1318</v>
+      </c>
+      <c r="F5">
+        <v>8255</v>
+      </c>
+      <c r="G5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6">
+        <v>336776</v>
+      </c>
+      <c r="E6">
+        <v>1021</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>141</v>
+      </c>
+      <c r="B7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7">
+        <v>336776</v>
+      </c>
+      <c r="E7">
+        <v>527</v>
+      </c>
+      <c r="F7">
+        <v>8255</v>
+      </c>
+      <c r="G7" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8">
+        <v>336776</v>
+      </c>
+      <c r="E8">
+        <v>1411</v>
+      </c>
+      <c r="F8">
+        <v>8713</v>
+      </c>
+      <c r="G8" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9">
+        <v>336776</v>
+      </c>
+      <c r="E9">
+        <v>1163</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>144</v>
+      </c>
+      <c r="B10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10">
+        <v>336776</v>
+      </c>
+      <c r="E10">
+        <v>577</v>
+      </c>
+      <c r="F10">
+        <v>9430</v>
+      </c>
+      <c r="G10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11">
+        <v>336776</v>
+      </c>
+      <c r="E11">
+        <v>16</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>145</v>
+      </c>
+      <c r="B12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12">
+        <v>336776</v>
+      </c>
+      <c r="E12">
+        <v>3844</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>146</v>
+      </c>
+      <c r="B13" t="s">
+        <v>131</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13">
+        <v>336776</v>
+      </c>
+      <c r="E13">
+        <v>4043</v>
+      </c>
+      <c r="F13">
+        <v>2512</v>
+      </c>
+      <c r="G13" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>147</v>
+      </c>
+      <c r="B14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14">
+        <v>336776</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>148</v>
+      </c>
+      <c r="B15" t="s">
+        <v>132</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15">
+        <v>336776</v>
+      </c>
+      <c r="E15">
+        <v>105</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>149</v>
+      </c>
+      <c r="B16" t="s">
+        <v>133</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16">
+        <v>336776</v>
+      </c>
+      <c r="E16">
+        <v>509</v>
+      </c>
+      <c r="F16">
+        <v>9430</v>
+      </c>
+      <c r="G16" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>150</v>
+      </c>
+      <c r="B17" t="s">
+        <v>134</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17">
+        <v>336776</v>
+      </c>
+      <c r="E17">
+        <v>214</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>151</v>
+      </c>
+      <c r="B18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18">
+        <v>336776</v>
+      </c>
+      <c r="E18">
+        <v>20</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>152</v>
+      </c>
+      <c r="B19" t="s">
+        <v>135</v>
+      </c>
+      <c r="C19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19">
+        <v>336776</v>
+      </c>
+      <c r="E19">
+        <v>60</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>153</v>
+      </c>
+      <c r="B20" t="s">
+        <v>109</v>
+      </c>
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20">
+        <v>336776</v>
+      </c>
+      <c r="E20">
+        <v>6936</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -1674,14 +2256,14 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.375" customWidth="1"/>
-    <col min="8" max="8" width="38.625" customWidth="1"/>
-    <col min="9" max="9" width="31.625" customWidth="1"/>
+    <col min="1" max="1" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.36328125" customWidth="1"/>
+    <col min="8" max="8" width="38.6328125" customWidth="1"/>
+    <col min="9" max="9" width="31.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="42" customHeight="1">
@@ -1713,7 +2295,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="66">
+    <row r="2" spans="1:9" ht="58">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -1740,7 +2322,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="71.25">
+    <row r="3" spans="1:9" ht="79">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -1764,7 +2346,7 @@
       </c>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="45.75">
+    <row r="4" spans="1:9" ht="41.5">
       <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
@@ -1788,7 +2370,7 @@
       </c>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:9" ht="45.75">
+    <row r="5" spans="1:9" ht="41.5">
       <c r="A5" s="3" t="s">
         <v>20</v>
       </c>
@@ -1812,7 +2394,7 @@
       </c>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" ht="27">
       <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
@@ -1836,7 +2418,7 @@
       </c>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:9" ht="49.5">
+    <row r="7" spans="1:9" ht="43.5">
       <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
@@ -1886,7 +2468,7 @@
       </c>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="58.5">
+    <row r="9" spans="1:9" ht="79">
       <c r="A9" s="3" t="s">
         <v>24</v>
       </c>
@@ -1927,11 +2509,11 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="52.125" customWidth="1"/>
+    <col min="2" max="2" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="52.08984375" customWidth="1"/>
     <col min="8" max="8" width="62" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1964,7 +2546,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" ht="29">
       <c r="A2" s="6" t="s">
         <v>44</v>
       </c>
@@ -1993,7 +2575,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" ht="29">
       <c r="A3" s="6" t="s">
         <v>47</v>
       </c>
@@ -2019,7 +2601,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="82.5">
+    <row r="4" spans="1:9" ht="72.5">
       <c r="A4" s="6" t="s">
         <v>49</v>
       </c>
@@ -2163,7 +2745,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="29.25">
+    <row r="10" spans="1:9" ht="29">
       <c r="A10" s="6" t="s">
         <v>51</v>
       </c>
@@ -2200,9 +2782,9 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="3" max="3" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="40" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2258,7 +2840,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="198">
+    <row r="3" spans="1:9" ht="174">
       <c r="A3" s="2" t="s">
         <v>76</v>
       </c>
@@ -2295,13 +2877,13 @@
       <selection activeCell="H10" activeCellId="1" sqref="F17 H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="20.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="59.75" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="59.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="42" customHeight="1">

</xml_diff>